<commit_message>
I added 2 functions: delete_user and most_mistakes
</commit_message>
<xml_diff>
--- a/Question_db_new.xlsx
+++ b/Question_db_new.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xxore\Documents\Project GitHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rotem\Documents\לימודים\שנה ב\Stark_Industries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9ABB16A-9C8B-48D5-8C84-237A77E8C47B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF67B33-408E-46C3-8FF5-D224A811536A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4116" yWindow="1224" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
@@ -444,18 +444,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
-    <col min="7" max="7" width="12.5546875" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" customWidth="1"/>
+    <col min="7" max="7" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -478,7 +478,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -494,11 +494,14 @@
       <c r="E2" t="s">
         <v>17</v>
       </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
       <c r="G2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -514,11 +517,14 @@
       <c r="E3" t="s">
         <v>17</v>
       </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
       <c r="G3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -534,11 +540,14 @@
       <c r="E4" t="s">
         <v>17</v>
       </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
       <c r="G4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -554,11 +563,14 @@
       <c r="E5" t="s">
         <v>17</v>
       </c>
+      <c r="F5">
+        <v>7</v>
+      </c>
       <c r="G5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -574,11 +586,14 @@
       <c r="E6" t="s">
         <v>17</v>
       </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
       <c r="G6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -594,11 +609,14 @@
       <c r="E7" t="s">
         <v>17</v>
       </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
       <c r="G7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -614,11 +632,14 @@
       <c r="E8" t="s">
         <v>17</v>
       </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
       <c r="G8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -634,11 +655,14 @@
       <c r="E9" t="s">
         <v>17</v>
       </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
       <c r="G9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -654,11 +678,14 @@
       <c r="E10" t="s">
         <v>17</v>
       </c>
+      <c r="F10">
+        <v>14</v>
+      </c>
       <c r="G10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -674,11 +701,14 @@
       <c r="E11" t="s">
         <v>17</v>
       </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
       <c r="G11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -694,11 +724,14 @@
       <c r="E12" t="s">
         <v>17</v>
       </c>
+      <c r="F12">
+        <v>8</v>
+      </c>
       <c r="G12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -714,11 +747,14 @@
       <c r="E13" t="s">
         <v>17</v>
       </c>
+      <c r="F13">
+        <v>12</v>
+      </c>
       <c r="G13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -734,11 +770,14 @@
       <c r="E14" t="s">
         <v>17</v>
       </c>
+      <c r="F14">
+        <v>9</v>
+      </c>
       <c r="G14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -754,11 +793,14 @@
       <c r="E15" t="s">
         <v>17</v>
       </c>
+      <c r="F15">
+        <v>7</v>
+      </c>
       <c r="G15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -773,6 +815,9 @@
       </c>
       <c r="E16" t="s">
         <v>17</v>
+      </c>
+      <c r="F16">
+        <v>6</v>
       </c>
       <c r="G16" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
choose category for the game
</commit_message>
<xml_diff>
--- a/Question_db_new.xlsx
+++ b/Question_db_new.xlsx
@@ -1,24 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amit\Desktop\update project\Stark_Industries\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA990F4-4DBB-4CE4-86E7-02E414BC23A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="22125" yWindow="3000" windowWidth="6675" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="28">
   <si>
-    <t>Unnamed: 0</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -98,17 +101,20 @@
   </si>
   <si>
     <t>Answer3</t>
+  </si>
+  <si>
+    <t>Index</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -116,7 +122,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -167,6 +173,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -213,7 +227,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -245,9 +259,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -279,6 +311,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -454,40 +504,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.25" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -495,28 +550,28 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H2">
         <v>5</v>
       </c>
       <c r="I2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -524,28 +579,28 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H3">
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -553,28 +608,28 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H4">
         <v>7</v>
       </c>
       <c r="I4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -582,28 +637,28 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H5">
         <v>4</v>
       </c>
       <c r="I5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -611,28 +666,28 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H6">
         <v>10</v>
       </c>
       <c r="I6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -640,28 +695,28 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -669,28 +724,28 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H8">
         <v>3</v>
       </c>
       <c r="I8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -698,28 +753,28 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H9">
         <v>14</v>
       </c>
       <c r="I9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -727,28 +782,28 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H10">
         <v>4</v>
       </c>
       <c r="I10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -756,28 +811,28 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H11">
         <v>8</v>
       </c>
       <c r="I11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -785,28 +840,28 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H12">
         <v>12</v>
       </c>
       <c r="I12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -814,28 +869,28 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H13">
         <v>9</v>
       </c>
       <c r="I13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -843,28 +898,28 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H14">
         <v>7</v>
       </c>
       <c r="I14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -872,25 +927,25 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H15">
         <v>6</v>
       </c>
       <c r="I15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
show the question in game function
</commit_message>
<xml_diff>
--- a/Question_db_new.xlsx
+++ b/Question_db_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amit\Desktop\update project\Stark_Industries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA990F4-4DBB-4CE4-86E7-02E414BC23A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2EE7227-D7CE-4644-AACC-FD894E127796}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22125" yWindow="3000" windowWidth="6675" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6735" yWindow="2610" windowWidth="11535" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="29">
   <si>
     <t>Category</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>Index</t>
+  </si>
+  <si>
+    <t>Question1</t>
   </si>
 </sst>
 </file>
@@ -505,15 +508,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -553,7 +561,7 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
         <v>24</v>
@@ -582,7 +590,7 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
         <v>24</v>
@@ -611,7 +619,7 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
         <v>24</v>
@@ -640,7 +648,7 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
@@ -666,10 +674,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
         <v>24</v>
@@ -698,7 +706,7 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
         <v>24</v>
@@ -710,7 +718,7 @@
         <v>26</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I7" t="s">
         <v>25</v>
@@ -727,7 +735,7 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
         <v>24</v>
@@ -739,10 +747,10 @@
         <v>26</v>
       </c>
       <c r="H8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -756,7 +764,7 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
         <v>24</v>
@@ -768,10 +776,10 @@
         <v>26</v>
       </c>
       <c r="H9">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="I9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -785,7 +793,7 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
         <v>24</v>
@@ -797,10 +805,10 @@
         <v>26</v>
       </c>
       <c r="H10">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="I10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -811,10 +819,10 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E11" t="s">
         <v>24</v>
@@ -826,10 +834,10 @@
         <v>26</v>
       </c>
       <c r="H11">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -843,7 +851,7 @@
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" t="s">
         <v>24</v>
@@ -855,10 +863,10 @@
         <v>26</v>
       </c>
       <c r="H12">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -872,7 +880,7 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
         <v>24</v>
@@ -884,10 +892,10 @@
         <v>26</v>
       </c>
       <c r="H13">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I13" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -901,7 +909,7 @@
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E14" t="s">
         <v>24</v>
@@ -913,7 +921,7 @@
         <v>26</v>
       </c>
       <c r="H14">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I14" t="s">
         <v>24</v>
@@ -930,23 +938,55 @@
         <v>9</v>
       </c>
       <c r="D15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15">
+        <v>7</v>
+      </c>
+      <c r="I15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
         <v>23</v>
       </c>
-      <c r="E15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H15">
+      <c r="E16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16">
         <v>6</v>
       </c>
-      <c r="I15" t="s">
-        <v>25</v>
-      </c>
+      <c r="I16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding question to data base
</commit_message>
<xml_diff>
--- a/Question_db_new.xlsx
+++ b/Question_db_new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eliormor/Desktop/Joy/Stark_Industries/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rotem\Documents\לימודים\שנה ב\Stark_Industries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B753845-8E0A-8643-9444-DEFC8C5A10E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA4C190-730D-45D7-8E0D-B5D8E8DDF119}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
   <si>
     <t>Category</t>
   </si>
@@ -64,12 +64,6 @@
     <t>Question4</t>
   </si>
   <si>
-    <t>Question5</t>
-  </si>
-  <si>
-    <t>Question10</t>
-  </si>
-  <si>
     <t>Answer1</t>
   </si>
   <si>
@@ -103,9 +97,6 @@
     <t>Tell them I'll do it later</t>
   </si>
   <si>
-    <t>Hit her</t>
-  </si>
-  <si>
     <t>Tell mom or dad</t>
   </si>
   <si>
@@ -185,6 +176,36 @@
   </si>
   <si>
     <t>Shout and rant</t>
+  </si>
+  <si>
+    <t>A friend from class is crying, what to do?</t>
+  </si>
+  <si>
+    <t>She is crying because she's sad, so I will ask her why she's sad</t>
+  </si>
+  <si>
+    <t>I don't know why she's crying so I'll leave her alone</t>
+  </si>
+  <si>
+    <t>Laugh because she looks funny</t>
+  </si>
+  <si>
+    <t>Yell at her</t>
+  </si>
+  <si>
+    <t>Play with her if I can because she wants my attention</t>
+  </si>
+  <si>
+    <t>My brother is hugging me but I don't like hugs, what do I do?</t>
+  </si>
+  <si>
+    <t>Push him away</t>
+  </si>
+  <si>
+    <t>Yell at him because he's annoying</t>
+  </si>
+  <si>
+    <t>Tell him that I know he means well but I don't like it</t>
   </si>
 </sst>
 </file>
@@ -195,7 +216,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -203,7 +224,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -266,7 +287,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -588,20 +609,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="243" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" customWidth="1"/>
-    <col min="5" max="5" width="14.5" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" customWidth="1"/>
+    <col min="6" max="6" width="17.1796875" customWidth="1"/>
+    <col min="7" max="7" width="8.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -624,7 +645,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -635,22 +656,22 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
         <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
       </c>
       <c r="G2">
         <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -661,22 +682,22 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
         <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -687,22 +708,22 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
         <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
       </c>
       <c r="G4">
         <v>7</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -713,22 +734,22 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
         <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>18</v>
       </c>
       <c r="G5">
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -736,25 +757,25 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="G6">
         <v>10</v>
       </c>
       <c r="H6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -762,25 +783,25 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
         <v>19</v>
-      </c>
-      <c r="F7" t="s">
-        <v>21</v>
       </c>
       <c r="G7">
         <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -788,25 +809,25 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
         <v>23</v>
       </c>
-      <c r="D8" t="s">
-        <v>25</v>
-      </c>
       <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" t="s">
         <v>24</v>
-      </c>
-      <c r="F8" t="s">
-        <v>26</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -814,25 +835,25 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="G9">
         <v>3</v>
       </c>
       <c r="H9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -840,25 +861,25 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G10">
         <v>14</v>
       </c>
       <c r="H10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -866,25 +887,25 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
       <c r="G11">
         <v>4</v>
       </c>
       <c r="H11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -892,25 +913,25 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
         <v>35</v>
       </c>
-      <c r="D12" t="s">
-        <v>38</v>
-      </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G12">
         <v>8</v>
       </c>
       <c r="H12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -918,25 +939,25 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" t="s">
         <v>39</v>
-      </c>
-      <c r="D13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" t="s">
-        <v>42</v>
       </c>
       <c r="G13">
         <v>12</v>
       </c>
       <c r="H13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -944,25 +965,25 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" t="s">
         <v>43</v>
-      </c>
-      <c r="D14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" t="s">
-        <v>46</v>
       </c>
       <c r="G14">
         <v>9</v>
       </c>
       <c r="H14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -970,25 +991,25 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" t="s">
         <v>47</v>
-      </c>
-      <c r="D15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" t="s">
-        <v>50</v>
       </c>
       <c r="G15">
         <v>7</v>
       </c>
       <c r="H15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -996,58 +1017,58 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" t="s">
         <v>51</v>
       </c>
-      <c r="D16" t="s">
-        <v>54</v>
-      </c>
       <c r="E16" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F16" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G16">
         <v>6</v>
       </c>
       <c r="H16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add comments to functions
</commit_message>
<xml_diff>
--- a/Question_db_new.xlsx
+++ b/Question_db_new.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rotem\Documents\לימודים\שנה ב\Stark_Industries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amit9530\Desktop\18.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A239B8-234B-47E8-9248-EAA671655B3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745162B2-5D92-42D6-8B38-B4D14C01E37B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -290,7 +290,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -612,21 +612,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="80.42578125" customWidth="1"/>
+    <col min="4" max="4" width="58.28515625" customWidth="1"/>
+    <col min="5" max="5" width="54.5703125" customWidth="1"/>
+    <col min="6" max="6" width="49.42578125" customWidth="1"/>
+    <col min="8" max="8" width="57.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -652,7 +653,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -678,7 +679,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -704,7 +705,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -730,7 +731,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -756,7 +757,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -782,7 +783,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -808,7 +809,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -834,7 +835,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -860,7 +861,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -886,7 +887,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -912,7 +913,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -938,7 +939,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -964,7 +965,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -990,7 +991,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1016,7 +1017,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Add 4 school questions
</commit_message>
<xml_diff>
--- a/Question_db_new.xlsx
+++ b/Question_db_new.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amit9530\Desktop\18.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xxore\Documents\Project GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745162B2-5D92-42D6-8B38-B4D14C01E37B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BCE0E1-F2C1-47E6-AC80-7E3AE4B30598}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="72">
   <si>
     <t>Category</t>
   </si>
@@ -52,30 +52,9 @@
     <t>Public Places</t>
   </si>
   <si>
-    <t>Question2</t>
-  </si>
-  <si>
-    <t>Question3</t>
-  </si>
-  <si>
-    <t>Question4</t>
-  </si>
-  <si>
-    <t>Answer1</t>
-  </si>
-  <si>
-    <t>Answer2</t>
-  </si>
-  <si>
-    <t>Answer3</t>
-  </si>
-  <si>
     <t>Index</t>
   </si>
   <si>
-    <t>Question1</t>
-  </si>
-  <si>
     <t>A friend from class is crying, what to do?</t>
   </si>
   <si>
@@ -209,6 +188,54 @@
   </si>
   <si>
     <t>Be polite and respect your relatives</t>
+  </si>
+  <si>
+    <t>What would you do if you need to go to the bathroom in mid class?</t>
+  </si>
+  <si>
+    <t>Just get out to the bathroom</t>
+  </si>
+  <si>
+    <t>Raise my hand and ask the teacher to go to the bathroom</t>
+  </si>
+  <si>
+    <t>Just shout to the teacher that I'm going to the bathroom</t>
+  </si>
+  <si>
+    <t>What would you do if you want to talk to your friend mid class?</t>
+  </si>
+  <si>
+    <t>Talk to him</t>
+  </si>
+  <si>
+    <t>I'll wait until the end of the class to tell him</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I'll pass a note and throw it </t>
+  </si>
+  <si>
+    <t>What would you do if someone threw something at you mid class?</t>
+  </si>
+  <si>
+    <t>I'll tell the teacher to handle it properly</t>
+  </si>
+  <si>
+    <t>I'll throw at back at them</t>
+  </si>
+  <si>
+    <t>I will shout "who threw this at me?!"</t>
+  </si>
+  <si>
+    <t>In recess someone pushed you, what would you do?</t>
+  </si>
+  <si>
+    <t>I'll tell him\her it wasn't nice and not to do it again</t>
+  </si>
+  <si>
+    <t>I'll insult him\her, so he\she won't do it again</t>
+  </si>
+  <si>
+    <t>I'll fight him\her to make him\her stop</t>
   </si>
 </sst>
 </file>
@@ -290,7 +317,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -613,23 +640,23 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="80.42578125" customWidth="1"/>
-    <col min="4" max="4" width="58.28515625" customWidth="1"/>
-    <col min="5" max="5" width="54.5703125" customWidth="1"/>
-    <col min="6" max="6" width="49.42578125" customWidth="1"/>
-    <col min="8" max="8" width="57.5703125" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="80.44140625" customWidth="1"/>
+    <col min="4" max="4" width="58.33203125" customWidth="1"/>
+    <col min="5" max="5" width="54.5546875" customWidth="1"/>
+    <col min="6" max="6" width="49.44140625" customWidth="1"/>
+    <col min="8" max="8" width="57.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -653,7 +680,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -661,25 +688,25 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="G2">
         <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -687,25 +714,25 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -713,25 +740,25 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="G4">
         <v>7</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -739,25 +766,25 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="G5">
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -765,25 +792,25 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G6">
         <v>10</v>
       </c>
       <c r="H6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -791,25 +818,25 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G7">
         <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -817,25 +844,25 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -843,25 +870,25 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="G9">
         <v>3</v>
       </c>
       <c r="H9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -869,25 +896,25 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G10">
         <v>14</v>
       </c>
       <c r="H10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -895,25 +922,25 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="F11" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="G11">
         <v>4</v>
       </c>
       <c r="H11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -921,25 +948,25 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F12" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="G12">
         <v>8</v>
       </c>
       <c r="H12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -947,25 +974,25 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E13" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F13" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="G13">
         <v>12</v>
       </c>
       <c r="H13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -973,25 +1000,25 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E14" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F14" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="G14">
         <v>9</v>
       </c>
       <c r="H14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -999,25 +1026,25 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F15" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="G15">
         <v>7</v>
       </c>
       <c r="H15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1025,22 +1052,22 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E16" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F16" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="G16">
         <v>6</v>
       </c>
       <c r="H16" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>